<commit_message>
FHIR-44320 remove strikethrough on MS
</commit_message>
<xml_diff>
--- a/input/images/In-Vitro At-Home Test V2 FHIR Mapping.xlsx
+++ b/input/images/In-Vitro At-Home Test V2 FHIR Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\HL7\FHIR\home-lab-report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\HL7\FHIR\home-lab-report\input\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F8EBBF-45DC-470F-BD6E-88C1E46E6A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363CBA4F-3330-4C89-941B-C3EC23B4C78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HL7v2 + FHIR" sheetId="1" r:id="rId1"/>
@@ -1557,7 +1557,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1597,6 +1597,12 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1650,7 +1656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1685,6 +1691,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1956,8 +1963,8 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3634,7 +3641,7 @@
       <c r="J34" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="16" t="s">
         <v>25</v>
       </c>
       <c r="L34" s="1" t="s">

</xml_diff>

<commit_message>
Fix up fsh warnings Update ignoreWarnings.txt Update mapping file
</commit_message>
<xml_diff>
--- a/input/images/In-Vitro At-Home Test V2 FHIR Mapping.xlsx
+++ b/input/images/In-Vitro At-Home Test V2 FHIR Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\HL7\FHIR\home-lab-report\input\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92197320-4914-4A67-9924-6BD1979AF9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCDDBBB-6FA6-48B1-9C28-21FE1325CFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HL7 V2 to FHIR" sheetId="3" r:id="rId1"/>
@@ -2481,7 +2481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF696548-21B4-4062-A0DF-3F383857234D}">
-  <dimension ref="A1:N206"/>
+  <dimension ref="A1:M206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -9507,6 +9507,26 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="9ed5a28f-e285-4793-933e-f86572ea3e88">
+      <UserInfo>
+        <DisplayName>Weitz, Andrew (NIH/NIBIB) [E]</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <LCG_x0020_Document_x0020_Workflow xmlns="4D6717E0-CDEB-44BF-A709-93EA007A7FBE">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007437C95740B27E489F4D6E839F8CF8B2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="143a829b742b703f123862b233d92dff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="4D6717E0-CDEB-44BF-A709-93EA007A7FBE" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="4d6717e0-cdeb-44bf-a709-93ea007a7fbe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35372c0a9306abecb7f01b69797803a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9723,26 +9743,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="9ed5a28f-e285-4793-933e-f86572ea3e88">
-      <UserInfo>
-        <DisplayName>Weitz, Andrew (NIH/NIBIB) [E]</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <LCG_x0020_Document_x0020_Workflow xmlns="4D6717E0-CDEB-44BF-A709-93EA007A7FBE">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6420E821-CCF6-4442-ACB4-DDE4A770B835}">
   <ds:schemaRefs>
@@ -9752,6 +9752,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71F1E9EE-CFA2-4828-A402-9D2D26481639}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
+    <ds:schemaRef ds:uri="4D6717E0-CDEB-44BF-A709-93EA007A7FBE"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76CE94C4-BFB3-484A-9445-0E2A40AF603D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9771,16 +9783,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71F1E9EE-CFA2-4828-A402-9D2D26481639}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
-    <ds:schemaRef ds:uri="4D6717E0-CDEB-44BF-A709-93EA007A7FBE"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>